<commit_message>
new version of system.
</commit_message>
<xml_diff>
--- a/deployment/appLocalization.xlsx
+++ b/deployment/appLocalization.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft.sharepoint.com/teams/ExtensesdoVivaLearning/Shared Documents/Viva Learning/1-Project Content/Viva Learning SharePoint Starter Kit/Learning and Development Suggestion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="511" documentId="8_{8E4B6140-EAB9-455C-8CE9-42A13AA2E32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{886A9A6A-9B47-4C98-A75E-48A2C8A9C069}"/>
+  <xr:revisionPtr revIDLastSave="518" documentId="8_{8E4B6140-EAB9-455C-8CE9-42A13AA2E32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5AE9657-F8BE-4AA8-A49F-5C8311D538E2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6311A743-8455-46E4-9529-7E7D8FEA940E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="188">
   <si>
     <t>ObjectName</t>
   </si>
@@ -509,9 +509,6 @@
     <t>fromSettingsPWID</t>
   </si>
   <si>
-    <t>ID do Power Apps</t>
-  </si>
-  <si>
     <t>Power Apps ID</t>
   </si>
   <si>
@@ -597,6 +594,12 @@
   </si>
   <si>
     <t>File Update</t>
+  </si>
+  <si>
+    <t>Teams Power Apps Link</t>
+  </si>
+  <si>
+    <t>Power Apps Teams Link</t>
   </si>
 </sst>
 </file>
@@ -652,10 +655,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E475E907-0EF1-48A3-A08D-4AD838729B91}" name="appLocalization" displayName="appLocalization" ref="A1:C125" totalsRowShown="0">
-  <autoFilter ref="A1:C125" xr:uid="{E475E907-0EF1-48A3-A08D-4AD838729B91}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C121">
-    <sortCondition ref="A1:A121"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E475E907-0EF1-48A3-A08D-4AD838729B91}" name="appLocalization" displayName="appLocalization" ref="A1:C126" totalsRowShown="0">
+  <autoFilter ref="A1:C126" xr:uid="{E475E907-0EF1-48A3-A08D-4AD838729B91}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C122">
+    <sortCondition ref="A1:A122"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{752FC097-B7E6-49A5-B58C-CC25EE939118}" name="ObjectName"/>
@@ -963,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA71E451-B8B7-453F-8A68-EE6DA4136A1E}">
-  <dimension ref="A1:C125"/>
+  <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,7 +1064,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1072,7 +1075,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1165,46 +1168,46 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>159</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
         <v>160</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
         <v>160</v>
-      </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1253,46 +1256,46 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>176</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
         <v>177</v>
-      </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>173</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
         <v>174</v>
-      </c>
-      <c r="B28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1369,18 +1372,18 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1388,21 +1391,21 @@
         <v>129</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1410,21 +1413,21 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1432,21 +1435,21 @@
         <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1454,21 +1457,21 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1476,43 +1479,43 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>168</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>169</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>167</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
         <v>168</v>
-      </c>
-      <c r="B48" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>167</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1520,21 +1523,21 @@
         <v>45</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1542,21 +1545,21 @@
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1564,21 +1567,21 @@
         <v>29</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1586,21 +1589,21 @@
         <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1608,21 +1611,21 @@
         <v>40</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C59" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1630,7 +1633,7 @@
         <v>38</v>
       </c>
       <c r="B60" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
         <v>39</v>
@@ -1638,35 +1641,35 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>171</v>
+        <v>38</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>172</v>
+        <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>170</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
         <v>171</v>
-      </c>
-      <c r="B62" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C63" t="s">
-        <v>58</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1674,21 +1677,21 @@
         <v>44</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1696,32 +1699,32 @@
         <v>80</v>
       </c>
       <c r="B66" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>156</v>
+        <v>80</v>
       </c>
       <c r="B67" t="s">
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1729,21 +1732,21 @@
         <v>120</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C69" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1751,21 +1754,21 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -1773,21 +1776,21 @@
         <v>64</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C74" t="s">
-        <v>134</v>
+        <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1795,21 +1798,21 @@
         <v>60</v>
       </c>
       <c r="B75" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>123</v>
+        <v>60</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -1817,21 +1820,21 @@
         <v>123</v>
       </c>
       <c r="B77" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C78" t="s">
-        <v>83</v>
+        <v>125</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -1839,21 +1842,21 @@
         <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>152</v>
+        <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>153</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -1861,21 +1864,21 @@
         <v>152</v>
       </c>
       <c r="B81" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>6</v>
+        <v>152</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>110</v>
+        <v>154</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -1883,7 +1886,7 @@
         <v>6</v>
       </c>
       <c r="B83" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C83" t="s">
         <v>110</v>
@@ -1891,13 +1894,13 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -1905,21 +1908,21 @@
         <v>51</v>
       </c>
       <c r="B85" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="B86" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C86" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -1927,21 +1930,21 @@
         <v>107</v>
       </c>
       <c r="B87" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -1949,21 +1952,21 @@
         <v>109</v>
       </c>
       <c r="B89" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C89" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -1971,21 +1974,21 @@
         <v>98</v>
       </c>
       <c r="B91" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -1993,21 +1996,21 @@
         <v>18</v>
       </c>
       <c r="B93" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>115</v>
+        <v>18</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C94" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -2015,21 +2018,21 @@
         <v>115</v>
       </c>
       <c r="B95" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="B96" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C96" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -2037,21 +2040,21 @@
         <v>65</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C97" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B98" t="s">
         <v>4</v>
       </c>
       <c r="C98" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -2059,21 +2062,21 @@
         <v>7</v>
       </c>
       <c r="B99" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>183</v>
+        <v>77</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="B100" t="s">
         <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -2081,21 +2084,21 @@
         <v>66</v>
       </c>
       <c r="B101" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B102" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
@@ -2103,21 +2106,21 @@
         <v>61</v>
       </c>
       <c r="B103" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C103" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="B104" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C104" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -2125,7 +2128,7 @@
         <v>111</v>
       </c>
       <c r="B105" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C105" t="s">
         <v>114</v>
@@ -2133,13 +2136,13 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C106" t="s">
-        <v>151</v>
+        <v>114</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -2147,21 +2150,21 @@
         <v>3</v>
       </c>
       <c r="B107" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C107" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>104</v>
+        <v>3</v>
       </c>
       <c r="B108" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C108" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
@@ -2169,21 +2172,21 @@
         <v>104</v>
       </c>
       <c r="B109" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C109" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="B110" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C110" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
@@ -2191,7 +2194,7 @@
         <v>8</v>
       </c>
       <c r="B111" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C111" t="s">
         <v>24</v>
@@ -2199,13 +2202,13 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C112" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -2213,21 +2216,21 @@
         <v>10</v>
       </c>
       <c r="B113" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C113" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C114" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -2235,21 +2238,21 @@
         <v>25</v>
       </c>
       <c r="B115" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B116" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C116" t="s">
-        <v>139</v>
+        <v>27</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -2257,21 +2260,21 @@
         <v>50</v>
       </c>
       <c r="B117" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C117" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B118" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C118" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -2279,21 +2282,21 @@
         <v>49</v>
       </c>
       <c r="B119" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C119" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="B120" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C120" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -2301,54 +2304,65 @@
         <v>9</v>
       </c>
       <c r="B121" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C121" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>180</v>
+        <v>9</v>
       </c>
       <c r="B122" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C122" t="s">
-        <v>181</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
+        <v>179</v>
+      </c>
+      <c r="B123" t="s">
+        <v>5</v>
+      </c>
+      <c r="C123" t="s">
         <v>180</v>
-      </c>
-      <c r="B123" t="s">
-        <v>4</v>
-      </c>
-      <c r="C123" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B124" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C124" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
+        <v>183</v>
+      </c>
+      <c r="B125" t="s">
+        <v>5</v>
+      </c>
+      <c r="C125" t="s">
         <v>184</v>
       </c>
-      <c r="B125" t="s">
-        <v>4</v>
-      </c>
-      <c r="C125" t="s">
-        <v>186</v>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>183</v>
+      </c>
+      <c r="B126" t="s">
+        <v>4</v>
+      </c>
+      <c r="C126" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2360,6 +2374,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="0d70a849-2114-4223-a5ad-92ccf221ce15" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1fcbaae4-82b5-419b-ae38-2eca790f6009">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010047D0094E1AFA924FABC361ECB6F17F21" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="56d990354425a93200d04157c413da13">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="1fcbaae4-82b5-419b-ae38-2eca790f6009" xmlns:ns3="0d70a849-2114-4223-a5ad-92ccf221ce15" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ee3267363721bacb982328efa233a1d9" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2593,29 +2629,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE705F7-37E7-4587-AD37-8D7532410CD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0d70a849-2114-4223-a5ad-92ccf221ce15" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1fcbaae4-82b5-419b-ae38-2eca790f6009">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A6D866-F97D-4C74-B4C9-04603A7627B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0d70a849-2114-4223-a5ad-92ccf221ce15"/>
+    <ds:schemaRef ds:uri="1fcbaae4-82b5-419b-ae38-2eca790f6009"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A716978-8384-43F0-B7AF-C33ADDBDDDDF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2635,26 +2669,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE705F7-37E7-4587-AD37-8D7532410CD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A6D866-F97D-4C74-B4C9-04603A7627B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0d70a849-2114-4223-a5ad-92ccf221ce15"/>
-    <ds:schemaRef ds:uri="1fcbaae4-82b5-419b-ae38-2eca790f6009"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>